<commit_message>
Add json input option
</commit_message>
<xml_diff>
--- a/src/examples/demo_inputs_transportation_facility_location.xlsx
+++ b/src/examples/demo_inputs_transportation_facility_location.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="16" documentId="8_{219022CE-CFFE-409A-9464-F800E6E350CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05C61AD0-9180-4E91-94E5-0E9764A51AD2}"/>
   <bookViews>
-    <workbookView xWindow="-15180" yWindow="-16320" windowWidth="29040" windowHeight="15720" firstSheet="11" activeTab="15" xr2:uid="{535FA824-8CF7-4082-B044-1F91AE1A9818}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23790" windowHeight="12050" firstSheet="11" activeTab="15" xr2:uid="{535FA824-8CF7-4082-B044-1F91AE1A9818}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="11" r:id="rId1"/>

</xml_diff>

<commit_message>
Add flow percentage constraints
</commit_message>
<xml_diff>
--- a/src/examples/demo_inputs_transportation_facility_location.xlsx
+++ b/src/examples/demo_inputs_transportation_facility_location.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\john-\Documents\Python Scripts\SupplyChainOptimizer\src\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83C62472-F763-4583-98A1-D04BB2D057D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{998773FD-103E-4954-B636-BBFF4F35C4FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-5520" windowWidth="38640" windowHeight="21120" xr2:uid="{535FA824-8CF7-4082-B044-1F91AE1A9818}"/>
+    <workbookView xWindow="-38520" yWindow="75" windowWidth="38640" windowHeight="21120" xr2:uid="{535FA824-8CF7-4082-B044-1F91AE1A9818}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="11" r:id="rId1"/>
@@ -9549,7 +9549,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>